<commit_message>
take screenshot and xml files
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/ecommerce.xlsx
+++ b/src/main/resources/testData/ecommerce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15640" activeTab="5"/>
+    <workbookView windowWidth="28000" windowHeight="15640" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="newUsers" sheetId="3" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="negativeLogin" sheetId="8" r:id="rId4"/>
     <sheet name="registerErrorMessages" sheetId="9" r:id="rId5"/>
     <sheet name="contactUs" sheetId="7" r:id="rId6"/>
+    <sheet name="searchKeywords" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382">
   <si>
     <t>title</t>
   </si>
@@ -1143,22 +1144,60 @@
   <si>
     <t>Hello, I would like to make another order of the same product</t>
   </si>
+  <si>
+    <t>searchKeyword</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>resultFound</t>
+  </si>
+  <si>
+    <t>t-shirt</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
+  </si>
+  <si>
+    <t>result has been found.</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>No results were found for your search</t>
+  </si>
+  <si>
+    <t>unicorns</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="d\-mm\-yyyy"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="d\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.75"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1202,7 +1241,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1217,8 +1256,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1233,15 +1288,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1265,14 +1312,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1286,7 +1333,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1297,14 +1344,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1329,13 +1368,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1353,25 +1488,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1383,79 +1518,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1467,37 +1536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1520,15 +1559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1540,6 +1570,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1573,23 +1618,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1613,156 +1652,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1771,10 +1813,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -2202,13 +2244,13 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>18395</v>
       </c>
       <c r="G2" t="s">
@@ -2235,7 +2277,7 @@
       <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="7">
         <v>12345</v>
       </c>
       <c r="P2" t="s">
@@ -2270,13 +2312,13 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>18396</v>
       </c>
       <c r="G3" t="s">
@@ -2303,7 +2345,7 @@
       <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="7">
         <v>12346</v>
       </c>
       <c r="P3" t="s">
@@ -2338,13 +2380,13 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>18397</v>
       </c>
       <c r="G4" t="s">
@@ -2371,7 +2413,7 @@
       <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="7">
         <v>12347</v>
       </c>
       <c r="P4" t="s">
@@ -2406,13 +2448,13 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>18398</v>
       </c>
       <c r="G5" t="s">
@@ -2439,7 +2481,7 @@
       <c r="N5" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="7">
         <v>12348</v>
       </c>
       <c r="P5" t="s">
@@ -2474,13 +2516,13 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>18399</v>
       </c>
       <c r="G6" t="s">
@@ -2507,7 +2549,7 @@
       <c r="N6" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="7">
         <v>12349</v>
       </c>
       <c r="P6" t="s">
@@ -2542,13 +2584,13 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>18400</v>
       </c>
       <c r="G7" t="s">
@@ -2575,7 +2617,7 @@
       <c r="N7" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="7">
         <v>12350</v>
       </c>
       <c r="P7" t="s">
@@ -2610,13 +2652,13 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>18401</v>
       </c>
       <c r="G8" t="s">
@@ -2643,7 +2685,7 @@
       <c r="N8" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="7">
         <v>12351</v>
       </c>
       <c r="P8" t="s">
@@ -2678,13 +2720,13 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>18402</v>
       </c>
       <c r="G9" t="s">
@@ -2711,7 +2753,7 @@
       <c r="N9" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="7">
         <v>12352</v>
       </c>
       <c r="P9" t="s">
@@ -2746,13 +2788,13 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E10" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>18403</v>
       </c>
       <c r="G10" t="s">
@@ -2779,7 +2821,7 @@
       <c r="N10" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="7">
         <v>12353</v>
       </c>
       <c r="P10" t="s">
@@ -2814,13 +2856,13 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>103</v>
       </c>
       <c r="E11" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>18404</v>
       </c>
       <c r="G11" t="s">
@@ -2847,7 +2889,7 @@
       <c r="N11" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="7">
         <v>12354</v>
       </c>
       <c r="P11" t="s">
@@ -2882,13 +2924,13 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E12" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>18405</v>
       </c>
       <c r="G12" t="s">
@@ -2915,7 +2957,7 @@
       <c r="N12" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="7">
         <v>12355</v>
       </c>
       <c r="P12" t="s">
@@ -2950,13 +2992,13 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>18406</v>
       </c>
       <c r="G13" t="s">
@@ -2983,7 +3025,7 @@
       <c r="N13" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="7">
         <v>12356</v>
       </c>
       <c r="P13" t="s">
@@ -3018,13 +3060,13 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>18407</v>
       </c>
       <c r="G14" t="s">
@@ -3051,7 +3093,7 @@
       <c r="N14" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="7">
         <v>12357</v>
       </c>
       <c r="P14" t="s">
@@ -3086,13 +3128,13 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>127</v>
       </c>
       <c r="E15" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>18408</v>
       </c>
       <c r="G15" t="s">
@@ -3119,7 +3161,7 @@
       <c r="N15" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="7">
         <v>12358</v>
       </c>
       <c r="P15" t="s">
@@ -3154,13 +3196,13 @@
       <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>133</v>
       </c>
       <c r="E16" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>18409</v>
       </c>
       <c r="G16" t="s">
@@ -3187,7 +3229,7 @@
       <c r="N16" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="7">
         <v>12359</v>
       </c>
       <c r="P16" t="s">
@@ -3222,13 +3264,13 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>139</v>
       </c>
       <c r="E17" t="s">
         <v>140</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>18410</v>
       </c>
       <c r="G17" t="s">
@@ -3255,7 +3297,7 @@
       <c r="N17" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="7">
         <v>12360</v>
       </c>
       <c r="P17" t="s">
@@ -3290,13 +3332,13 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>145</v>
       </c>
       <c r="E18" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>18411</v>
       </c>
       <c r="G18" t="s">
@@ -3323,7 +3365,7 @@
       <c r="N18" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="7">
         <v>12361</v>
       </c>
       <c r="P18" t="s">
@@ -3358,13 +3400,13 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>151</v>
       </c>
       <c r="E19" t="s">
         <v>152</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>18412</v>
       </c>
       <c r="G19" t="s">
@@ -3391,7 +3433,7 @@
       <c r="N19" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="7">
         <v>12362</v>
       </c>
       <c r="P19" t="s">
@@ -3426,13 +3468,13 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6">
         <v>18413</v>
       </c>
       <c r="G20" t="s">
@@ -3459,7 +3501,7 @@
       <c r="N20" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="7">
         <v>12363</v>
       </c>
       <c r="P20" t="s">
@@ -3494,13 +3536,13 @@
       <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>163</v>
       </c>
       <c r="E21" t="s">
         <v>164</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6">
         <v>18414</v>
       </c>
       <c r="G21" t="s">
@@ -3527,7 +3569,7 @@
       <c r="N21" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="7">
         <v>12364</v>
       </c>
       <c r="P21" t="s">
@@ -3562,13 +3604,13 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>169</v>
       </c>
       <c r="E22" t="s">
         <v>170</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6">
         <v>18415</v>
       </c>
       <c r="G22" t="s">
@@ -3595,7 +3637,7 @@
       <c r="N22" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="7">
         <v>12365</v>
       </c>
       <c r="P22" t="s">
@@ -3630,13 +3672,13 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>175</v>
       </c>
       <c r="E23" t="s">
         <v>176</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>18416</v>
       </c>
       <c r="G23" t="s">
@@ -3663,7 +3705,7 @@
       <c r="N23" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="7">
         <v>12366</v>
       </c>
       <c r="P23" t="s">
@@ -3698,13 +3740,13 @@
       <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>181</v>
       </c>
       <c r="E24" t="s">
         <v>182</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>18417</v>
       </c>
       <c r="G24" t="s">
@@ -3731,7 +3773,7 @@
       <c r="N24" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="7">
         <v>12367</v>
       </c>
       <c r="P24" t="s">
@@ -3766,13 +3808,13 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>187</v>
       </c>
       <c r="E25" t="s">
         <v>188</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>18418</v>
       </c>
       <c r="G25" t="s">
@@ -3799,7 +3841,7 @@
       <c r="N25" t="s">
         <v>33</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="7">
         <v>12368</v>
       </c>
       <c r="P25" t="s">
@@ -3834,13 +3876,13 @@
       <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>193</v>
       </c>
       <c r="E26" t="s">
         <v>194</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6">
         <v>18419</v>
       </c>
       <c r="G26" t="s">
@@ -3867,7 +3909,7 @@
       <c r="N26" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="7">
         <v>12369</v>
       </c>
       <c r="P26" t="s">
@@ -3902,13 +3944,13 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>199</v>
       </c>
       <c r="E27" t="s">
         <v>200</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6">
         <v>18420</v>
       </c>
       <c r="G27" t="s">
@@ -3935,7 +3977,7 @@
       <c r="N27" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="7">
         <v>12370</v>
       </c>
       <c r="P27" t="s">
@@ -3970,13 +4012,13 @@
       <c r="C28" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>205</v>
       </c>
       <c r="E28" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6">
         <v>18421</v>
       </c>
       <c r="G28" t="s">
@@ -4003,7 +4045,7 @@
       <c r="N28" t="s">
         <v>33</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="7">
         <v>12371</v>
       </c>
       <c r="P28" t="s">
@@ -4038,13 +4080,13 @@
       <c r="C29" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>211</v>
       </c>
       <c r="E29" t="s">
         <v>212</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6">
         <v>18422</v>
       </c>
       <c r="G29" t="s">
@@ -4071,7 +4113,7 @@
       <c r="N29" t="s">
         <v>33</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="7">
         <v>12372</v>
       </c>
       <c r="P29" t="s">
@@ -4106,13 +4148,13 @@
       <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E30" t="s">
         <v>218</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6">
         <v>18423</v>
       </c>
       <c r="G30" t="s">
@@ -4139,7 +4181,7 @@
       <c r="N30" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="7">
         <v>12373</v>
       </c>
       <c r="P30" t="s">
@@ -4174,13 +4216,13 @@
       <c r="C31" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>223</v>
       </c>
       <c r="E31" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="6">
         <v>18424</v>
       </c>
       <c r="G31" t="s">
@@ -4207,7 +4249,7 @@
       <c r="N31" t="s">
         <v>33</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="7">
         <v>12374</v>
       </c>
       <c r="P31" t="s">
@@ -4242,13 +4284,13 @@
       <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>229</v>
       </c>
       <c r="E32" t="s">
         <v>230</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="6">
         <v>18425</v>
       </c>
       <c r="G32" t="s">
@@ -4275,7 +4317,7 @@
       <c r="N32" t="s">
         <v>33</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="7">
         <v>12375</v>
       </c>
       <c r="P32" t="s">
@@ -4310,13 +4352,13 @@
       <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>235</v>
       </c>
       <c r="E33" t="s">
         <v>236</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="6">
         <v>18426</v>
       </c>
       <c r="G33" t="s">
@@ -4343,7 +4385,7 @@
       <c r="N33" t="s">
         <v>33</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="7">
         <v>12376</v>
       </c>
       <c r="P33" t="s">
@@ -4378,13 +4420,13 @@
       <c r="C34" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>241</v>
       </c>
       <c r="E34" t="s">
         <v>242</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="6">
         <v>18427</v>
       </c>
       <c r="G34" t="s">
@@ -4411,7 +4453,7 @@
       <c r="N34" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="7">
         <v>12377</v>
       </c>
       <c r="P34" t="s">
@@ -4446,13 +4488,13 @@
       <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>247</v>
       </c>
       <c r="E35" t="s">
         <v>248</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="6">
         <v>18428</v>
       </c>
       <c r="G35" t="s">
@@ -4479,7 +4521,7 @@
       <c r="N35" t="s">
         <v>33</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="7">
         <v>12378</v>
       </c>
       <c r="P35" t="s">
@@ -4514,13 +4556,13 @@
       <c r="C36" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E36" t="s">
         <v>254</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="6">
         <v>18429</v>
       </c>
       <c r="G36" t="s">
@@ -4547,7 +4589,7 @@
       <c r="N36" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="7">
         <v>12379</v>
       </c>
       <c r="P36" t="s">
@@ -4582,13 +4624,13 @@
       <c r="C37" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>259</v>
       </c>
       <c r="E37" t="s">
         <v>260</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="6">
         <v>18430</v>
       </c>
       <c r="G37" t="s">
@@ -4615,7 +4657,7 @@
       <c r="N37" t="s">
         <v>33</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="7">
         <v>12380</v>
       </c>
       <c r="P37" t="s">
@@ -4650,13 +4692,13 @@
       <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>265</v>
       </c>
       <c r="E38" t="s">
         <v>266</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="6">
         <v>18431</v>
       </c>
       <c r="G38" t="s">
@@ -4683,7 +4725,7 @@
       <c r="N38" t="s">
         <v>33</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="7">
         <v>12381</v>
       </c>
       <c r="P38" t="s">
@@ -4718,13 +4760,13 @@
       <c r="C39" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>271</v>
       </c>
       <c r="E39" t="s">
         <v>272</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="6">
         <v>18432</v>
       </c>
       <c r="G39" t="s">
@@ -4751,7 +4793,7 @@
       <c r="N39" t="s">
         <v>33</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="7">
         <v>12382</v>
       </c>
       <c r="P39" t="s">
@@ -4786,13 +4828,13 @@
       <c r="C40" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>277</v>
       </c>
       <c r="E40" t="s">
         <v>278</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="6">
         <v>18433</v>
       </c>
       <c r="G40" t="s">
@@ -4819,7 +4861,7 @@
       <c r="N40" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="7">
         <v>12383</v>
       </c>
       <c r="P40" t="s">
@@ -4854,13 +4896,13 @@
       <c r="C41" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>283</v>
       </c>
       <c r="E41" t="s">
         <v>284</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6">
         <v>18434</v>
       </c>
       <c r="G41" t="s">
@@ -4887,7 +4929,7 @@
       <c r="N41" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="7">
         <v>12384</v>
       </c>
       <c r="P41" t="s">
@@ -4922,13 +4964,13 @@
       <c r="C42" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>289</v>
       </c>
       <c r="E42" t="s">
         <v>290</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="6">
         <v>18435</v>
       </c>
       <c r="G42" t="s">
@@ -4955,7 +4997,7 @@
       <c r="N42" t="s">
         <v>33</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="7">
         <v>12385</v>
       </c>
       <c r="P42" t="s">
@@ -4990,13 +5032,13 @@
       <c r="C43" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>295</v>
       </c>
       <c r="E43" t="s">
         <v>296</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="6">
         <v>18436</v>
       </c>
       <c r="G43" t="s">
@@ -5023,7 +5065,7 @@
       <c r="N43" t="s">
         <v>33</v>
       </c>
-      <c r="O43" s="6">
+      <c r="O43" s="7">
         <v>12386</v>
       </c>
       <c r="P43" t="s">
@@ -5058,13 +5100,13 @@
       <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>301</v>
       </c>
       <c r="E44" t="s">
         <v>302</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="6">
         <v>18437</v>
       </c>
       <c r="G44" t="s">
@@ -5091,7 +5133,7 @@
       <c r="N44" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="7">
         <v>12387</v>
       </c>
       <c r="P44" t="s">
@@ -5126,13 +5168,13 @@
       <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="5" t="s">
         <v>307</v>
       </c>
       <c r="E45" t="s">
         <v>308</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="6">
         <v>18438</v>
       </c>
       <c r="G45" t="s">
@@ -5159,7 +5201,7 @@
       <c r="N45" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="7">
         <v>12388</v>
       </c>
       <c r="P45" t="s">
@@ -5194,13 +5236,13 @@
       <c r="C46" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>313</v>
       </c>
       <c r="E46" t="s">
         <v>314</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="6">
         <v>18439</v>
       </c>
       <c r="G46" t="s">
@@ -5227,7 +5269,7 @@
       <c r="N46" t="s">
         <v>33</v>
       </c>
-      <c r="O46" s="6">
+      <c r="O46" s="7">
         <v>12389</v>
       </c>
       <c r="P46" t="s">
@@ -5262,13 +5304,13 @@
       <c r="C47" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>319</v>
       </c>
       <c r="E47" t="s">
         <v>320</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="6">
         <v>18440</v>
       </c>
       <c r="G47" t="s">
@@ -5295,7 +5337,7 @@
       <c r="N47" t="s">
         <v>33</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="7">
         <v>12390</v>
       </c>
       <c r="P47" t="s">
@@ -5330,13 +5372,13 @@
       <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>325</v>
       </c>
       <c r="E48" t="s">
         <v>326</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="6">
         <v>18441</v>
       </c>
       <c r="G48" t="s">
@@ -5363,7 +5405,7 @@
       <c r="N48" t="s">
         <v>33</v>
       </c>
-      <c r="O48" s="6">
+      <c r="O48" s="7">
         <v>12391</v>
       </c>
       <c r="P48" t="s">
@@ -5398,13 +5440,13 @@
       <c r="C49" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="5" t="s">
         <v>331</v>
       </c>
       <c r="E49" t="s">
         <v>332</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="6">
         <v>18442</v>
       </c>
       <c r="G49" t="s">
@@ -5431,7 +5473,7 @@
       <c r="N49" t="s">
         <v>33</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O49" s="7">
         <v>12392</v>
       </c>
       <c r="P49" t="s">
@@ -5466,13 +5508,13 @@
       <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>337</v>
       </c>
       <c r="E50" t="s">
         <v>338</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="6">
         <v>18443</v>
       </c>
       <c r="G50" t="s">
@@ -5499,7 +5541,7 @@
       <c r="N50" t="s">
         <v>33</v>
       </c>
-      <c r="O50" s="6">
+      <c r="O50" s="7">
         <v>12393</v>
       </c>
       <c r="P50" t="s">
@@ -5584,13 +5626,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="22.5625" customWidth="1"/>
   </cols>
@@ -5604,87 +5646,16 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>343</v>
       </c>
       <c r="B2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>343</v>
-      </c>
-      <c r="B3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>343</v>
-      </c>
-      <c r="B4" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>343</v>
-      </c>
-      <c r="B5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>343</v>
-      </c>
-      <c r="B6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>343</v>
-      </c>
-      <c r="B7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>343</v>
-      </c>
-      <c r="B8" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>343</v>
-      </c>
-      <c r="B9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>343</v>
-      </c>
-      <c r="B10" t="s">
-        <v>344</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A8" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A7" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A6" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A5" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId1" display="kevinlee1234@gmail.com"/>
-    <hyperlink ref="A10" r:id="rId1" display="kevinlee1234@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="kevinlee1234@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -5715,7 +5686,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>346</v>
       </c>
       <c r="B2" t="s">
@@ -5723,15 +5694,15 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>349</v>
       </c>
       <c r="B4" t="s">
@@ -5777,7 +5748,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>343</v>
       </c>
       <c r="B2" t="s">
@@ -5807,7 +5778,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>343</v>
       </c>
       <c r="C5" t="s">
@@ -5844,7 +5815,7 @@
       </c>
     </row>
     <row r="2" ht="126" spans="1:1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5859,7 +5830,7 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+    <sheetView zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5896,7 +5867,7 @@
       <c r="A2" t="s">
         <v>362</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>363</v>
       </c>
       <c r="C2" t="s">
@@ -5916,7 +5887,7 @@
       <c r="A3" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>368</v>
       </c>
       <c r="C3" t="s">
@@ -5936,7 +5907,7 @@
       <c r="A4" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>343</v>
       </c>
       <c r="D4" t="s">
@@ -5958,4 +5929,81 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="246" zoomScaleNormal="246" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="14.0625" customWidth="1"/>
+    <col min="2" max="2" width="33.1875" customWidth="1"/>
+    <col min="3" max="3" width="18.1875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" t="s">
+        <v>380</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hover over, scroll down and some ehancements
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/ecommerce.xlsx
+++ b/src/main/resources/testData/ecommerce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="15640" firstSheet="2" activeTab="6"/>
+    <workbookView windowWidth="28000" windowHeight="14840" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="newUsers" sheetId="3" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="registerErrorMessages" sheetId="9" r:id="rId5"/>
     <sheet name="contactUs" sheetId="7" r:id="rId6"/>
     <sheet name="searchKeywords" sheetId="10" r:id="rId7"/>
+    <sheet name="dresses" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387">
   <si>
     <t>title</t>
   </si>
@@ -1174,17 +1175,32 @@
   <si>
     <t>unicorns</t>
   </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>dresses</t>
+  </si>
+  <si>
+    <t>t-shirts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-shirts,blouses,casual dresses,evening dresses,summer dresses </t>
+  </si>
+  <si>
+    <t>casual dresses,evening dresses, summer dresses</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="d\-mm\-yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="d\-mm\-yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1226,6 +1242,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1241,10 +1265,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1258,37 +1289,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1312,19 +1312,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1333,15 +1357,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1362,7 +1378,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1374,31 +1540,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1410,133 +1552,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,11 +1566,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1589,6 +1620,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1618,32 +1658,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1652,142 +1668,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1816,7 +1832,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -2143,7 +2159,7 @@
   <sheetPr/>
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+    <sheetView zoomScale="143" zoomScaleNormal="143" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -5936,8 +5952,8 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="246" zoomScaleNormal="246" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="246" zoomScaleNormal="246" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -6006,4 +6022,44 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="59.5625" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>